<commit_message>
Fixing fitur import, at template
</commit_message>
<xml_diff>
--- a/POS/public/template_kategori.xlsx
+++ b/POS/public/template_kategori.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/PWL_2025/week8/PWL_POS/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/PWL_2025/POS/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6ECA5D4-D6E5-6243-AC1D-FDE602F3B14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398F9624-B09D-D34D-B2F2-1F3EACF52432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21120" yWindow="4880" windowWidth="10000" windowHeight="7100" xr2:uid="{5B0AFC75-281F-9F41-92F5-D21F86155B3C}"/>
   </bookViews>
@@ -403,7 +403,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -425,7 +425,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>